<commit_message>
update AHPANP tutorial example
</commit_message>
<xml_diff>
--- a/Examples/AhpAnpTutorialCarModel/Excel_AHP_Car_selection_Excel_results.xlsx
+++ b/Examples/AhpAnpTutorialCarModel/Excel_AHP_Car_selection_Excel_results.xlsx
@@ -17,6 +17,7 @@
     <sheet name="Graph Model2" sheetId="8" state="visible" r:id="rId8"/>
     <sheet name="Graph Model3" sheetId="9" state="visible" r:id="rId9"/>
     <sheet name="Graph Model4" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="Graph Model5" sheetId="11" state="visible" r:id="rId11"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -470,6 +471,39 @@
 </wsDr>
 </file>
 
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="11801475" cy="3705225"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2175,6 +2209,13 @@
         <color rgb="ff0b30b5"/>
       </dataBar>
     </cfRule>
+    <cfRule type="dataBar" priority="41">
+      <dataBar showValue="1">
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="ff0b30b5"/>
+      </dataBar>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I13:I15">
     <cfRule type="dataBar" priority="1">
@@ -2212,6 +2253,13 @@
         <color rgb="ff0b30b5"/>
       </dataBar>
     </cfRule>
+    <cfRule type="dataBar" priority="41">
+      <dataBar showValue="1">
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="ff0b30b5"/>
+      </dataBar>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I21:I23">
     <cfRule type="dataBar" priority="1">
@@ -2249,6 +2297,13 @@
         <color rgb="ff0b30b5"/>
       </dataBar>
     </cfRule>
+    <cfRule type="dataBar" priority="41">
+      <dataBar showValue="1">
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="ff0b30b5"/>
+      </dataBar>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I29:I31">
     <cfRule type="dataBar" priority="1">
@@ -2286,6 +2341,13 @@
         <color rgb="ff0b30b5"/>
       </dataBar>
     </cfRule>
+    <cfRule type="dataBar" priority="41">
+      <dataBar showValue="1">
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="ff0b30b5"/>
+      </dataBar>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I37:I39">
     <cfRule type="dataBar" priority="1">
@@ -2323,6 +2385,13 @@
         <color rgb="ff0b30b5"/>
       </dataBar>
     </cfRule>
+    <cfRule type="dataBar" priority="41">
+      <dataBar showValue="1">
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="ff0b30b5"/>
+      </dataBar>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I45:I47">
     <cfRule type="dataBar" priority="1">
@@ -2360,6 +2429,13 @@
         <color rgb="ff0b30b5"/>
       </dataBar>
     </cfRule>
+    <cfRule type="dataBar" priority="41">
+      <dataBar showValue="1">
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="ff0b30b5"/>
+      </dataBar>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I53:I55">
     <cfRule type="dataBar" priority="1">
@@ -2397,6 +2473,13 @@
         <color rgb="ff0b30b5"/>
       </dataBar>
     </cfRule>
+    <cfRule type="dataBar" priority="41">
+      <dataBar showValue="1">
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="ff0b30b5"/>
+      </dataBar>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I61:I63">
     <cfRule type="dataBar" priority="1">
@@ -2428,6 +2511,13 @@
       </dataBar>
     </cfRule>
     <cfRule type="dataBar" priority="33">
+      <dataBar showValue="1">
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="ff0b30b5"/>
+      </dataBar>
+    </cfRule>
+    <cfRule type="dataBar" priority="41">
       <dataBar showValue="1">
         <cfvo type="min" val="0"/>
         <cfvo type="max" val="0"/>
@@ -2440,6 +2530,25 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>